<commit_message>
additional example showing how to implement self paced reading
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>color</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>resp</t>
   </si>
   <si>
@@ -35,6 +38,12 @@
   </si>
   <si>
     <t>[255, 0, 0]</t>
+  </si>
+  <si>
+    <t>instr_resp</t>
+  </si>
+  <si>
+    <t>stroop_response</t>
   </si>
   <si>
     <t>green</t>
@@ -401,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,118 +429,142 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>1082.300000009127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <v>1640.499999979511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>119</v>
       </c>
-      <c r="D3">
-        <v>1617.300000041723</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>168.7999999849126</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>260.4999999748543</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>113</v>
+      </c>
+      <c r="E4">
+        <v>331.6999999806285</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
         <v>119</v>
       </c>
-      <c r="D5">
-        <v>251.8999999156222</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>249.8999999370426</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
         <v>119</v>
       </c>
-      <c r="D6">
-        <v>1617.300000041723</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>168.7999999849126</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>260.4999999748543</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>113</v>
+      </c>
+      <c r="E7">
+        <v>331.6999999806285</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <v>119</v>
       </c>
-      <c r="D8">
-        <v>251.8999999156222</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
+      <c r="E8">
+        <v>249.8999999370426</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>